<commit_message>
cleaning up monthly data and date times
</commit_message>
<xml_diff>
--- a/raw/Daily_Weather_Raw_2017-Present.xlsx
+++ b/raw/Daily_Weather_Raw_2017-Present.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandriapawlik/Documents/Research/EDI/UMBS_Weather_Data/Raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandriapawlik/Documents/Research/EDI/UMBS_Weather_Data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84F3F352-B327-0B41-A156-E7B02D56BAFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C71AA5-2AD2-9E4E-AD39-442EA2E7A1F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="27660" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="460" windowWidth="27660" windowHeight="17540" firstSheet="6" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="May20" sheetId="1" r:id="rId1"/>
@@ -9684,7 +9684,7 @@
   </sheetPr>
   <dimension ref="A1:Q906"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -20283,7 +20283,9 @@
   </sheetPr>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21397,7 +21399,7 @@
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
       <c r="F33">
         <f t="shared" ref="F33:H33" si="0">SUM(F2:F32)</f>
@@ -21412,8 +21414,8 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="16" t="s">
         <v>282</v>
       </c>
     </row>
@@ -22593,7 +22595,9 @@
   </sheetPr>
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -32607,7 +32611,9 @@
   </sheetPr>
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -42421,7 +42427,9 @@
   </sheetPr>
   <dimension ref="A1:Q936"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>